<commit_message>
on application close and start restore the initial variable values fix
</commit_message>
<xml_diff>
--- a/energyPowerOptimization/energy_optimization.xlsx
+++ b/energyPowerOptimization/energy_optimization.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" fullCalcOnLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Produs</t>
   </si>
@@ -52,13 +52,65 @@
   </si>
   <si>
     <t>optimizareTurbinaEoliana</t>
+  </si>
+  <si>
+    <t>Frigider</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>146</t>
+  </si>
+  <si>
+    <t>2525.8</t>
+  </si>
+  <si>
+    <t>1841.425</t>
+  </si>
+  <si>
+    <t>Prajitor Paine</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>730</t>
+  </si>
+  <si>
+    <t>Televizor</t>
+  </si>
+  <si>
+    <t>12.6</t>
+  </si>
+  <si>
+    <t>153.3</t>
+  </si>
+  <si>
+    <t>Aspirator</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>1752</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -369,62 +421,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="A2:I6"/>
+      <selection activeCell="H7" sqref="A2:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="1" width="15.85546875" customWidth="1"/>
     <col min="2" max="2" width="10.140625" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" bestFit="1" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" bestFit="1" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" bestFit="1" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" bestFit="1" width="22.7109375" customWidth="1"/>
+    <col min="9" max="9" bestFit="1" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="0" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="0">
+        <v>6</v>
+      </c>
+      <c r="F2" s="0">
+        <v>252.6</v>
+      </c>
+      <c r="G2" s="0">
+        <v>3073.3</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
@@ -433,5 +556,6 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>